<commit_message>
Completed question 2 and first part of question 3
</commit_message>
<xml_diff>
--- a/Execution Time Data.xlsx
+++ b/Execution Time Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcitz\Desktop\McGill\ECSE420\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{060D715F-D9E8-423C-AFA0-D637BDE78285}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C068A575-2D25-4ECA-A2C9-0CF4A9AF9844}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{514E7C7A-9D69-4581-91C5-912AA5DC0A2C}"/>
   </bookViews>
@@ -2770,7 +2770,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>